<commit_message>
Fixed typo in BOM. Thanks, @hitmanmcc!
</commit_message>
<xml_diff>
--- a/BOM-N64_RGB_Amp.xlsx
+++ b/BOM-N64_RGB_Amp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tzorrimahm/Desktop/GitHub/N64_RGB_Amp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tzorrimahm/Downloads/N64_RGB_Amp-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6569295-9506-2E47-97AC-1BEE323A801E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D17E2F-9093-5142-AD09-99A9716EA560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="960" windowWidth="27840" windowHeight="16160" xr2:uid="{3551FF10-B2C5-004D-97D2-89E9084F1538}"/>
+    <workbookView xWindow="960" yWindow="520" windowWidth="27840" windowHeight="16160" xr2:uid="{3551FF10-B2C5-004D-97D2-89E9084F1538}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>C11</t>
   </si>
   <si>
-    <t>C21, C31, C31</t>
-  </si>
-  <si>
     <t>https://www.mouser.de/ProductDetail/Texas-Instruments/THS7374IPWR?qs=qU0TI%2FZyA%252BxCw%252BZ%2FnXjpBw%3D%3D</t>
   </si>
   <si>
@@ -231,13 +228,16 @@
   </si>
   <si>
     <t>https://www.mouser.de/ProjectManager/ProjectDetail.aspx?AccessID=139e1f6c21</t>
+  </si>
+  <si>
+    <t>C21, C31, C41</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -624,7 +624,7 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
@@ -634,17 +634,17 @@
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24">
+    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -662,7 +662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -679,102 +679,102 @@
         <v>16</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -785,136 +785,136 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>